<commit_message>
trouble reading excel files: freshly created files solves problem
problem with needing to specify numeric format even when cell is numeric Reading a character 1 for caseID for normal case

reading a whole bunch of NaN in TRUTH sheet for  incorrectCaseIDsInTP.xlsx
</commit_message>
<xml_diff>
--- a/extdata/toyFiles/FROC/bad/frocCr2BlankRows.xlsx
+++ b/extdata/toyFiles/FROC/bad/frocCr2BlankRows.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10111"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/RJafroc/inst/extdata/toyFiles/FROC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Dev/GitHub/PyJafroc/extdata/toyFiles/FROC/bad/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B2B487-4141-ED4B-84A3-0F9CB7C8D5A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307F28DE-DD08-3942-89E5-45E1D750D57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13720" yWindow="1140" windowWidth="10440" windowHeight="10080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13720" yWindow="1140" windowWidth="10440" windowHeight="10080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="TP" sheetId="3" r:id="rId1"/>
-    <sheet name="FP" sheetId="2" r:id="rId2"/>
+    <sheet name="LL" sheetId="3" r:id="rId1"/>
+    <sheet name="NL" sheetId="2" r:id="rId2"/>
     <sheet name="TRUTH" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="10">
   <si>
     <t>CaseID</t>
   </si>
@@ -52,9 +52,6 @@
     <t>ModalityID</t>
   </si>
   <si>
-    <t>FP_Rating</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -64,22 +61,10 @@
     <t>2</t>
   </si>
   <si>
-    <t>TP_Rating</t>
+    <t>LLRating</t>
   </si>
   <si>
-    <t>0,1,2</t>
-  </si>
-  <si>
-    <t>0,1</t>
-  </si>
-  <si>
-    <t>Paradigm</t>
-  </si>
-  <si>
-    <t>FROC</t>
-  </si>
-  <si>
-    <t>FCTRL</t>
+    <t>NLRating</t>
   </si>
 </sst>
 </file>
@@ -580,7 +565,7 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -603,19 +588,19 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M1">
         <f ca="1">RAND()-0.5</f>
-        <v>0.2582387784166974</v>
+        <v>-0.19076552552066228</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1">
         <v>70</v>
@@ -628,19 +613,19 @@
       </c>
       <c r="J2">
         <f t="shared" ref="J2:J5" ca="1" si="0">ROUND(0.5*(RAND()-0.5)+E2, 2)</f>
-        <v>5.39</v>
+        <v>5.05</v>
       </c>
       <c r="M2">
         <f t="shared" ref="M2:M13" ca="1" si="1">RAND()-0.5</f>
-        <v>0.23264078500560392</v>
+        <v>-0.30777879272297426</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>70</v>
@@ -653,19 +638,19 @@
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5199999999999996</v>
+        <v>4.57</v>
       </c>
       <c r="M3">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.8059593184847871E-2</v>
+        <v>5.2824782788023938E-2</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>71</v>
@@ -678,19 +663,19 @@
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>2.81</v>
+        <v>3.03</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.34316099353964247</v>
+        <v>0.26916028014694859</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1">
         <v>72</v>
@@ -703,19 +688,19 @@
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2</v>
+        <v>6.05</v>
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="1"/>
-        <v>0.28850397828423724</v>
+        <v>0.17262188369744513</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1">
         <v>73</v>
@@ -728,19 +713,19 @@
       </c>
       <c r="J6">
         <f t="shared" ref="J6:J11" ca="1" si="2">ROUND(0.5*(RAND()-0.5)+E6, 2)</f>
-        <v>4.9400000000000004</v>
+        <v>5.07</v>
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.41458417368488032</v>
+        <v>0.21990721171633099</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>73</v>
@@ -753,19 +738,19 @@
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="2"/>
-        <v>5.1100000000000003</v>
+        <v>5.29</v>
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.18122780411291217</v>
+        <v>-0.12957856237896004</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1">
         <v>74</v>
@@ -778,19 +763,19 @@
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="2"/>
-        <v>4.16</v>
+        <v>4.5</v>
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.31524822807274155</v>
+        <v>-0.33032862293570331</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1">
         <v>70</v>
@@ -803,19 +788,19 @@
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="2"/>
-        <v>4.97</v>
+        <v>5.3</v>
       </c>
       <c r="M9">
         <f t="shared" ca="1" si="1"/>
-        <v>0.34784777738853223</v>
+        <v>0.272786393160383</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1">
         <v>71</v>
@@ -828,19 +813,19 @@
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="2"/>
-        <v>3.44</v>
+        <v>3.41</v>
       </c>
       <c r="M10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.26444759919425775</v>
+        <v>0.47213680431678395</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1">
         <v>72</v>
@@ -853,19 +838,19 @@
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="2"/>
-        <v>4.68</v>
+        <v>4.6900000000000004</v>
       </c>
       <c r="M11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2482425623523391</v>
+        <v>-0.19041556255198555</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1">
         <v>72</v>
@@ -878,15 +863,15 @@
       </c>
       <c r="M12">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.21209662582215327</v>
+        <v>-0.2727056758685622</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1">
         <v>72</v>
@@ -899,15 +884,15 @@
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="1"/>
-        <v>2.8936979237050853E-3</v>
+        <v>-0.46845055635910859</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" s="1">
         <v>73</v>
@@ -921,10 +906,10 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" s="1">
         <v>74</v>
@@ -937,15 +922,15 @@
       </c>
       <c r="M15">
         <f ca="1">AVERAGE(M1:M13)</f>
-        <v>9.8798277037073137E-3</v>
+        <v>-3.3121995577849277E-2</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="1">
         <v>70</v>
@@ -959,10 +944,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" s="1">
         <v>71</v>
@@ -976,10 +961,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="1">
         <v>72</v>
@@ -993,10 +978,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" s="1">
         <v>73</v>
@@ -1010,10 +995,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" s="1">
         <v>74</v>
@@ -1027,10 +1012,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" s="1">
         <v>70</v>
@@ -1044,10 +1029,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" s="1">
         <v>71</v>
@@ -1061,10 +1046,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" s="1">
         <v>72</v>
@@ -1078,10 +1063,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C24" s="1">
         <v>73</v>
@@ -1095,10 +1080,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25" s="1">
         <v>74</v>
@@ -1112,10 +1097,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26" s="1">
         <v>70</v>
@@ -1129,10 +1114,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" s="1">
         <v>71</v>
@@ -1146,10 +1131,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C28" s="1">
         <v>72</v>
@@ -1163,10 +1148,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C29" s="1">
         <v>73</v>
@@ -1180,10 +1165,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C30" s="1">
         <v>74</v>
@@ -1197,10 +1182,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C31" s="1">
         <v>70</v>
@@ -1214,10 +1199,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C32" s="1">
         <v>71</v>
@@ -1244,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1265,15 +1250,15 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -1283,15 +1268,15 @@
       </c>
       <c r="J2">
         <f t="shared" ref="J2:J11" ca="1" si="0">ROUND(0.5*(RAND()-0.5)+D2, 2)</f>
-        <v>1.19</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -1301,15 +1286,15 @@
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="0"/>
-        <v>2.27</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>2</v>
@@ -1319,15 +1304,15 @@
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="0"/>
-        <v>2.34</v>
+        <v>2.4500000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1">
         <v>3</v>
@@ -1337,15 +1322,15 @@
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.82</v>
+        <v>1.91</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -1355,15 +1340,15 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="0"/>
-        <v>1.99</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -1373,15 +1358,15 @@
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="0"/>
-        <v>3.22</v>
+        <v>2.88</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1">
         <v>2</v>
@@ -1392,10 +1377,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1">
         <v>3</v>
@@ -1405,15 +1390,15 @@
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.15</v>
+        <v>2.16</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
@@ -1423,15 +1408,15 @@
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -1441,15 +1426,15 @@
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="0"/>
-        <v>1.88</v>
+        <v>2.19</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1">
         <v>3</v>
@@ -1460,10 +1445,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
@@ -1474,10 +1459,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C14" s="1">
         <v>2</v>
@@ -1488,10 +1473,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C15" s="1">
         <v>74</v>
@@ -1502,10 +1487,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="1">
         <v>73</v>
@@ -1516,10 +1501,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" s="1">
         <v>3</v>
@@ -1530,10 +1515,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
@@ -1544,10 +1529,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1">
         <v>2</v>
@@ -1558,10 +1543,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" s="1">
         <v>3</v>
@@ -1572,10 +1557,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" s="1">
         <v>71</v>
@@ -1586,10 +1571,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" s="1">
         <v>71</v>
@@ -1600,10 +1585,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" s="1">
         <v>72</v>
@@ -1625,21 +1610,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="8.83203125" style="1"/>
-    <col min="4" max="4" width="13" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1649,17 +1631,8 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1669,17 +1642,8 @@
       <c r="C2" s="2">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1689,17 +1653,8 @@
       <c r="C3" s="2">
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1709,15 +1664,8 @@
       <c r="C4" s="2">
         <v>0</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>70</v>
       </c>
@@ -1727,31 +1675,18 @@
       <c r="C5" s="3">
         <v>0.3</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>70</v>
       </c>
@@ -1761,15 +1696,8 @@
       <c r="C8" s="3">
         <v>0.7</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>71</v>
       </c>
@@ -1779,15 +1707,8 @@
       <c r="C9" s="2">
         <v>1</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>72</v>
       </c>
@@ -1797,15 +1718,8 @@
       <c r="C10" s="2">
         <v>0.33300000000000002</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>72</v>
       </c>
@@ -1815,15 +1729,8 @@
       <c r="C11" s="2">
         <v>0.33300000000000002</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>72</v>
       </c>
@@ -1833,15 +1740,8 @@
       <c r="C12" s="2">
         <v>0.33300000000000002</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>73</v>
       </c>
@@ -1851,15 +1751,8 @@
       <c r="C13" s="3">
         <v>0.1</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>73</v>
       </c>
@@ -1869,15 +1762,8 @@
       <c r="C14" s="3">
         <v>0.9</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>74</v>
       </c>
@@ -1887,104 +1773,71 @@
       <c r="C15" s="2">
         <v>1</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>